<commit_message>
corrected s to S
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_H.BROWN_12.11.20.xlsx
+++ b/bioSample/bioSample_H.BROWN_12.11.20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/bioSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CF10DDC-C61A-1343-ACDA-77862A522D32}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F766141-24FC-F043-8247-FC293C0A46EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2540" yWindow="4620" windowWidth="27640" windowHeight="14860" xr2:uid="{EE012232-8892-A34E-801F-20204B1E3992}"/>
   </bookViews>
@@ -33,18 +33,12 @@
     <t>harvester</t>
   </si>
   <si>
-    <t>biosampleNumber</t>
-  </si>
-  <si>
     <t>experimentDesign</t>
   </si>
   <si>
     <t>strain</t>
   </si>
   <si>
-    <t>genotype</t>
-  </si>
-  <si>
     <t>inductionDelay</t>
   </si>
   <si>
@@ -91,6 +85,12 @@
   </si>
   <si>
     <t>CO2</t>
+  </si>
+  <si>
+    <t>genotype1</t>
+  </si>
+  <si>
+    <t>bioSampleNumber</t>
   </si>
 </sst>
 </file>
@@ -445,10 +445,15 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="21.1640625" customWidth="1"/>
+    <col min="4" max="4" width="25.83203125" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -458,57 +463,57 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>6</v>
-      </c>
-      <c r="K1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
       </c>
       <c r="H2">
         <v>30</v>
@@ -525,25 +530,25 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
         <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
       </c>
       <c r="H3">
         <v>30</v>
@@ -560,31 +565,31 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
         <v>14</v>
       </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
       <c r="H4">
         <v>30</v>
       </c>
       <c r="I4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -598,31 +603,31 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
         <v>14</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
       </c>
       <c r="H5">
         <v>37</v>
       </c>
       <c r="I5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -636,31 +641,31 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H6">
         <v>30</v>
       </c>
       <c r="I6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -674,31 +679,31 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H7">
         <v>37</v>
       </c>
       <c r="I7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -712,31 +717,31 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H8">
         <v>30</v>
       </c>
       <c r="I8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -750,31 +755,31 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H9">
         <v>37</v>
       </c>
       <c r="I9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -788,31 +793,31 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" t="s">
         <v>14</v>
       </c>
-      <c r="F10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" t="s">
-        <v>16</v>
-      </c>
       <c r="H10">
         <v>30</v>
       </c>
       <c r="I10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -826,31 +831,31 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" t="s">
         <v>14</v>
-      </c>
-      <c r="F11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" t="s">
-        <v>16</v>
       </c>
       <c r="H11">
         <v>37</v>
       </c>
       <c r="I11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -864,31 +869,31 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H12">
         <v>30</v>
       </c>
       <c r="I12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -902,31 +907,31 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C13">
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H13">
         <v>37</v>
       </c>
       <c r="I13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -940,31 +945,31 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C14">
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H14">
         <v>30</v>
       </c>
       <c r="I14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -978,31 +983,31 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C15">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H15">
         <v>37</v>
       </c>
       <c r="I15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -1016,31 +1021,31 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C16">
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" t="s">
         <v>14</v>
       </c>
-      <c r="F16" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" t="s">
-        <v>16</v>
-      </c>
       <c r="H16">
         <v>30</v>
       </c>
       <c r="I16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -1054,31 +1059,31 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C17">
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" t="s">
         <v>14</v>
-      </c>
-      <c r="F17" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" t="s">
-        <v>16</v>
       </c>
       <c r="H17">
         <v>37</v>
       </c>
       <c r="I17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J17">
         <v>0</v>
@@ -1092,31 +1097,31 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C18">
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H18">
         <v>30</v>
       </c>
       <c r="I18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J18">
         <v>0</v>
@@ -1130,31 +1135,31 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C19">
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H19">
         <v>37</v>
       </c>
       <c r="I19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J19">
         <v>0</v>
@@ -1168,31 +1173,31 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C20">
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G20" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H20">
         <v>30</v>
       </c>
       <c r="I20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J20">
         <v>0</v>
@@ -1206,31 +1211,31 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C21">
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E21" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F21" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G21" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H21">
         <v>37</v>
       </c>
       <c r="I21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J21">
         <v>0</v>
@@ -1244,31 +1249,31 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C22">
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" t="s">
         <v>14</v>
       </c>
-      <c r="F22" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" t="s">
-        <v>16</v>
-      </c>
       <c r="H22">
         <v>30</v>
       </c>
       <c r="I22" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J22">
         <v>0</v>
@@ -1282,31 +1287,31 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C23">
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" t="s">
         <v>14</v>
-      </c>
-      <c r="F23" t="s">
-        <v>11</v>
-      </c>
-      <c r="G23" t="s">
-        <v>16</v>
       </c>
       <c r="H23">
         <v>37</v>
       </c>
       <c r="I23" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J23">
         <v>0</v>
@@ -1320,31 +1325,31 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C24">
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E24" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F24" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G24" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H24">
         <v>30</v>
       </c>
       <c r="I24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J24">
         <v>0</v>
@@ -1358,31 +1363,31 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C25">
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E25" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F25" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H25">
         <v>37</v>
       </c>
       <c r="I25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J25">
         <v>0</v>
@@ -1396,31 +1401,31 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C26">
         <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G26" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H26">
         <v>30</v>
       </c>
       <c r="I26" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J26">
         <v>0</v>
@@ -1434,31 +1439,31 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C27">
         <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E27" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F27" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G27" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H27">
         <v>37</v>
       </c>
       <c r="I27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J27">
         <v>0</v>

</xml_diff>

<commit_message>
fixing typos in column headings
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_H.BROWN_12.11.20.xlsx
+++ b/bioSample/bioSample_H.BROWN_12.11.20.xlsx
@@ -37,7 +37,7 @@
     <t xml:space="preserve">strain</t>
   </si>
   <si>
-    <t xml:space="preserve">genotype</t>
+    <t xml:space="preserve">genotype1</t>
   </si>
   <si>
     <t xml:space="preserve">medium</t>
@@ -186,7 +186,7 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>